<commit_message>
removed deprecated terms and listed them in Annex
- The deprecated terms have been removed (consent relations)
- A list of deprecated terms has been added to DPV, DPV-SKOS, and
  DPV-OWL along with information on removal as well as alternatives
- This resolves#15 regarding anonymisation concepts being structed based
  on DeIdentification as the parent
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/legal_basis.xlsx
+++ b/documentation-generator/vocab_csv/legal_basis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="254">
   <si>
     <t>Term</t>
   </si>
@@ -817,7 +817,10 @@
     <t>Generic property specifying when or under which condition(s) the consent will expire</t>
   </si>
   <si>
-    <t>sunset</t>
+    <t>use dpv:hasDuration instead</t>
+  </si>
+  <si>
+    <t>deprecated</t>
   </si>
   <si>
     <t xml:space="preserve">Harshvardhan J. Pandit, Mark Lizar, Bud Bruegger
@@ -845,9 +848,6 @@
     <t>Specifies the condition or event that determines the expiry of consent</t>
   </si>
   <si>
-    <t>Can be TextOrDocumentOrURI</t>
-  </si>
-  <si>
     <t>hasProvisionMethod</t>
   </si>
   <si>
@@ -857,7 +857,7 @@
     <t>Specifies the method by which consent was provisioned or provided</t>
   </si>
   <si>
-    <t>Can be used to record information of how consent was provided e.g. by a click to a form, in writing, etc., by logging into a system and confirm per email, or with some additional authentication, etc.</t>
+    <t>use dpv:hasIndicationMethod instead</t>
   </si>
   <si>
     <t>hasProvisionTime</t>
@@ -869,6 +869,9 @@
     <t>Specifies the instant in time when consent was given</t>
   </si>
   <si>
+    <t>use dpv:isIndicatedAtTime instead</t>
+  </si>
+  <si>
     <t>hasWithdrawalMethod</t>
   </si>
   <si>
@@ -878,9 +881,6 @@
     <t>Specifries the method by which consent can be/has been withdrawn</t>
   </si>
   <si>
-    <t>Can be used to record information of how to withdraw consent, e.g. by a click to a form, in writing, etc., by logging into a system and confirm per email, or with some additional authentication, etc.</t>
-  </si>
-  <si>
     <t>hasWithdrawalTime</t>
   </si>
   <si>
@@ -902,7 +902,7 @@
     <t>dpv:LegalEntity</t>
   </si>
   <si>
-    <t>Normally this would be the dataSubject, but in some exceptional cases, the consent might be withdraawn on behalf by someone else, e.g. parents of minors.</t>
+    <t>use dpv:isIndicatedBy instead</t>
   </si>
   <si>
     <t>hasProvisionBy</t>
@@ -914,9 +914,6 @@
     <t>Specifies the entity that provisioned or provided consent</t>
   </si>
   <si>
-    <t>Normally this would be the dataSubject, but in some exceptional cases, the consent might be given on behalf by someone else, e.g. parents of minors.</t>
-  </si>
-  <si>
     <t>hasProvisionByJustification</t>
   </si>
   <si>
@@ -926,7 +923,7 @@
     <t>Specifies the justification for entity providing consent</t>
   </si>
   <si>
-    <t>This field can be used to proivde a justification why the provision was provided by another DataSubject or legal entity,  e.g. declariing the relationship (parent, guardian), in combination with the field provisionBy</t>
+    <t>use dpv:hasJustification instead</t>
   </si>
   <si>
     <t>hasWithdrawalByJustification</t>
@@ -938,9 +935,6 @@
     <t>Specifies the justification for entity withdrawing consent</t>
   </si>
   <si>
-    <t>This field can be used to proivde a justification why the weithdrawal was done by another DataSubject or legal entity, e.g. declariing the relationship (parent, guardian), in combination with the field withdrawalBy</t>
-  </si>
-  <si>
     <t>hasConsentNotice</t>
   </si>
   <si>
@@ -950,7 +944,7 @@
     <t>Specifies the notice provided in context of consent</t>
   </si>
   <si>
-    <t>The actual notice that the Data Subject received to consent to, either a text or link to a document, which should be usable to decide whether the form or consent was compliant to legislation, e.g. documenting how the user has been informed about rights and implications (such as, right to data portability,right to recitffy, right to erasure, right to restrict processing, right to object, rights regarding automated decision making or profiling, processors, third parties, sub-processors, outside-EEA transfers, automated decision-making, or other necessary details of the privacy-policy). Can be TextOrDocumentOrURI.</t>
+    <t>use dpv:hasNotice instead</t>
   </si>
   <si>
     <t>isExplicit</t>
@@ -965,7 +959,7 @@
     <t>xsd:boolean</t>
   </si>
   <si>
-    <t>The conditions for what is considered 'explicit consent' differ by norms and laws.</t>
+    <t>use dpv:ExplicitlyExpressedConsent instead</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1109,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1209,6 +1203,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -3959,139 +3956,88 @@
       <c r="C8" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
+      <c r="I8" s="19" t="s">
+        <v>206</v>
+      </c>
       <c r="K8" s="22">
         <v>43560.0</v>
       </c>
       <c r="L8" s="22">
-        <v>44734.0</v>
+        <v>44899.0</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N8" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O8" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="20"/>
-      <c r="AB8" s="20"/>
     </row>
     <row r="9">
       <c r="A9" s="19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
+        <v>211</v>
+      </c>
       <c r="F9" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
+        <v>212</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>206</v>
+      </c>
       <c r="K9" s="22">
         <v>43560.0</v>
       </c>
-      <c r="L9" s="22">
-        <v>44734.0</v>
+      <c r="L9" s="32">
+        <v>44899.0</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N9" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O9" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20"/>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="20"/>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="20"/>
-      <c r="Z9" s="20"/>
-      <c r="AA9" s="20"/>
-      <c r="AB9" s="20"/>
     </row>
     <row r="10">
       <c r="A10" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="J10" s="20"/>
+      <c r="I10" s="29" t="s">
+        <v>206</v>
+      </c>
       <c r="K10" s="22">
         <v>43560.0</v>
       </c>
       <c r="L10" s="22">
-        <v>44734.0</v>
+        <v>44899.0</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N10" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O10" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="20"/>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
     </row>
     <row r="11">
       <c r="A11" s="19" t="s">
@@ -4103,43 +4049,24 @@
       <c r="C11" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="32" t="s">
+      <c r="I11" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="J11" s="20"/>
       <c r="K11" s="22">
         <v>43560.0</v>
       </c>
-      <c r="L11" s="22">
-        <v>44734.0</v>
+      <c r="L11" s="32">
+        <v>44899.0</v>
       </c>
       <c r="M11" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N11" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O11" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="20"/>
-      <c r="U11" s="20"/>
-      <c r="V11" s="20"/>
-      <c r="W11" s="20"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="20"/>
-      <c r="Z11" s="20"/>
-      <c r="AA11" s="20"/>
-      <c r="AB11" s="20"/>
     </row>
     <row r="12">
       <c r="A12" s="19" t="s">
@@ -4151,89 +4078,53 @@
       <c r="C12" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
+      <c r="I12" s="19" t="s">
+        <v>223</v>
+      </c>
       <c r="K12" s="22">
         <v>43560.0</v>
       </c>
       <c r="L12" s="22">
-        <v>44734.0</v>
+        <v>44899.0</v>
       </c>
       <c r="M12" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O12" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="20"/>
-      <c r="U12" s="20"/>
-      <c r="V12" s="20"/>
-      <c r="W12" s="20"/>
-      <c r="X12" s="20"/>
-      <c r="Y12" s="20"/>
-      <c r="Z12" s="20"/>
-      <c r="AA12" s="20"/>
-      <c r="AB12" s="20"/>
     </row>
     <row r="13">
       <c r="A13" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="J13" s="20"/>
+      <c r="I13" s="33" t="s">
+        <v>219</v>
+      </c>
       <c r="K13" s="22">
         <v>43560.0</v>
       </c>
-      <c r="L13" s="22">
-        <v>44734.0</v>
+      <c r="L13" s="32">
+        <v>44899.0</v>
       </c>
       <c r="M13" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O13" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
-      <c r="T13" s="20"/>
-      <c r="U13" s="20"/>
-      <c r="V13" s="20"/>
-      <c r="W13" s="20"/>
-      <c r="X13" s="20"/>
-      <c r="Y13" s="20"/>
-      <c r="Z13" s="20"/>
-      <c r="AA13" s="20"/>
-      <c r="AB13" s="20"/>
     </row>
     <row r="14">
       <c r="A14" s="19" t="s">
@@ -4245,41 +4136,24 @@
       <c r="C14" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
+      <c r="I14" s="19" t="s">
+        <v>223</v>
+      </c>
       <c r="K14" s="22">
         <v>43560.0</v>
       </c>
       <c r="L14" s="22">
-        <v>44734.0</v>
+        <v>44899.0</v>
       </c>
       <c r="M14" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O14" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="20"/>
-      <c r="V14" s="20"/>
-      <c r="W14" s="20"/>
-      <c r="X14" s="20"/>
-      <c r="Y14" s="20"/>
-      <c r="Z14" s="20"/>
-      <c r="AA14" s="20"/>
-      <c r="AB14" s="20"/>
     </row>
     <row r="15">
       <c r="A15" s="19" t="s">
@@ -4291,45 +4165,27 @@
       <c r="C15" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="D15" s="20"/>
       <c r="E15" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
       <c r="I15" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="J15" s="20"/>
       <c r="K15" s="22">
         <v>43560.0</v>
       </c>
-      <c r="L15" s="22">
-        <v>44734.0</v>
+      <c r="L15" s="32">
+        <v>44899.0</v>
       </c>
       <c r="M15" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O15" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="20"/>
-      <c r="U15" s="20"/>
-      <c r="V15" s="20"/>
-      <c r="W15" s="20"/>
-      <c r="X15" s="20"/>
-      <c r="Y15" s="20"/>
-      <c r="Z15" s="20"/>
-      <c r="AA15" s="20"/>
-      <c r="AB15" s="20"/>
     </row>
     <row r="16">
       <c r="A16" s="19" t="s">
@@ -4341,239 +4197,172 @@
       <c r="C16" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="D16" s="20"/>
       <c r="E16" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="19" t="s">
-        <v>238</v>
-      </c>
-      <c r="J16" s="20"/>
+      <c r="I16" s="29" t="s">
+        <v>234</v>
+      </c>
       <c r="K16" s="22">
         <v>43560.0</v>
       </c>
       <c r="L16" s="22">
-        <v>44734.0</v>
+        <v>44899.0</v>
       </c>
       <c r="M16" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N16" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O16" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
-      <c r="T16" s="20"/>
-      <c r="U16" s="20"/>
-      <c r="V16" s="20"/>
-      <c r="W16" s="20"/>
-      <c r="X16" s="20"/>
-      <c r="Y16" s="20"/>
-      <c r="Z16" s="20"/>
-      <c r="AA16" s="20"/>
-      <c r="AB16" s="20"/>
     </row>
     <row r="17">
       <c r="A17" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="B17" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="C17" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="I17" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="33" t="s">
-        <v>242</v>
-      </c>
-      <c r="J17" s="20"/>
       <c r="K17" s="22">
         <v>43560.0</v>
       </c>
-      <c r="L17" s="22">
-        <v>44734.0</v>
+      <c r="L17" s="32">
+        <v>44899.0</v>
       </c>
       <c r="M17" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O17" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="34"/>
-      <c r="T17" s="34"/>
-      <c r="U17" s="34"/>
-      <c r="V17" s="34"/>
-      <c r="W17" s="34"/>
-      <c r="X17" s="34"/>
-      <c r="Y17" s="34"/>
-      <c r="Z17" s="34"/>
-      <c r="AA17" s="34"/>
-      <c r="AB17" s="34"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="35"/>
+      <c r="W17" s="35"/>
+      <c r="X17" s="35"/>
+      <c r="Y17" s="35"/>
+      <c r="Z17" s="35"/>
+      <c r="AA17" s="35"/>
+      <c r="AB17" s="35"/>
     </row>
     <row r="18">
       <c r="A18" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="B18" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="C18" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>245</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="33" t="s">
-        <v>246</v>
-      </c>
-      <c r="J18" s="20"/>
+      <c r="I18" s="29" t="s">
+        <v>241</v>
+      </c>
       <c r="K18" s="22">
         <v>43560.0</v>
       </c>
       <c r="L18" s="22">
-        <v>44734.0</v>
+        <v>44899.0</v>
       </c>
       <c r="M18" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O18" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="34"/>
-      <c r="U18" s="34"/>
-      <c r="V18" s="34"/>
-      <c r="W18" s="34"/>
-      <c r="X18" s="34"/>
-      <c r="Y18" s="34"/>
-      <c r="Z18" s="34"/>
-      <c r="AA18" s="34"/>
-      <c r="AB18" s="34"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="35"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="35"/>
+      <c r="X18" s="35"/>
+      <c r="Y18" s="35"/>
+      <c r="Z18" s="35"/>
+      <c r="AA18" s="35"/>
+      <c r="AB18" s="35"/>
     </row>
     <row r="19">
       <c r="A19" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="I19" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>249</v>
-      </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="19" t="s">
-        <v>250</v>
-      </c>
-      <c r="J19" s="20"/>
       <c r="K19" s="22">
         <v>43560.0</v>
       </c>
-      <c r="L19" s="22">
-        <v>44734.0</v>
+      <c r="L19" s="32">
+        <v>44899.0</v>
       </c>
       <c r="M19" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N19" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O19" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20"/>
-      <c r="U19" s="20"/>
-      <c r="V19" s="20"/>
-      <c r="W19" s="20"/>
-      <c r="X19" s="20"/>
-      <c r="Y19" s="20"/>
-      <c r="Z19" s="20"/>
-      <c r="AA19" s="20"/>
-      <c r="AB19" s="20"/>
     </row>
     <row r="20">
       <c r="A20" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="E20" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="I20" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="J20" s="20"/>
       <c r="K20" s="22">
         <v>43560.0</v>
       </c>
       <c r="L20" s="22">
-        <v>44734.0</v>
+        <v>44899.0</v>
       </c>
       <c r="M20" s="19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O20" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
-      <c r="U20" s="20"/>
-      <c r="V20" s="20"/>
-      <c r="W20" s="20"/>
-      <c r="X20" s="20"/>
-      <c r="Y20" s="20"/>
-      <c r="Z20" s="20"/>
-      <c r="AA20" s="20"/>
-      <c r="AB20" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:AB20">

</xml_diff>